<commit_message>
Update client feedback about export & email template
</commit_message>
<xml_diff>
--- a/ADMIN/mau_xuat_excel.xlsx
+++ b/ADMIN/mau_xuat_excel.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>STT</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>DANH SÁCH KHÁCH HÀNG ĐẶT VÉ QUA WEDSITE</t>
+  </si>
+  <si>
+    <t>Mã khách hàng</t>
   </si>
 </sst>
 </file>
@@ -494,26 +497,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="17.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -523,9 +527,10 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="33" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -533,27 +538,30 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>